<commit_message>
POM page object model added in project
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/employedata.xlsx
+++ b/src/test/resources/testData/employedata.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\6 Cucumber\mavenProject19-12-2023\babarMaven\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311A8E28-7E01-490D-BB09-4B1D985C5C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2EC756-5F30-4760-B224-19AC0C9DD61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="7875" xr2:uid="{B37AE323-F7E0-4FD7-9150-A67EB1EAC2F8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B37AE323-F7E0-4FD7-9150-A67EB1EAC2F8}"/>
   </bookViews>
   <sheets>
-    <sheet name="employeData" sheetId="1" r:id="rId1"/>
+    <sheet name="list" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,43 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
-  <si>
-    <t>babar1</t>
-  </si>
-  <si>
-    <t>babar2</t>
-  </si>
-  <si>
-    <t>babar3</t>
-  </si>
-  <si>
-    <t>abcxyz</t>
-  </si>
-  <si>
-    <t>babar4</t>
-  </si>
-  <si>
-    <t>babar5</t>
-  </si>
-  <si>
-    <t>babar6</t>
-  </si>
-  <si>
-    <t>lmnopq</t>
-  </si>
-  <si>
-    <t>babar7</t>
-  </si>
-  <si>
-    <t>babar8</t>
-  </si>
-  <si>
-    <t>babar9</t>
-  </si>
-  <si>
-    <t>xxxyyy</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>firstName</t>
   </si>
@@ -78,29 +42,56 @@
     <t>password</t>
   </si>
   <si>
-    <t>aaAA12345</t>
-  </si>
-  <si>
-    <t>hhHH98765</t>
-  </si>
-  <si>
-    <t>jJJ102983</t>
-  </si>
-  <si>
-    <t>aag43vlkAA12345</t>
-  </si>
-  <si>
-    <t>hhHv4oo3H98765</t>
-  </si>
-  <si>
-    <t>jJJ102kl3ffw983</t>
+    <t>babar14</t>
+  </si>
+  <si>
+    <t>babar26</t>
+  </si>
+  <si>
+    <t>babar38</t>
+  </si>
+  <si>
+    <t>abcxyz83</t>
+  </si>
+  <si>
+    <t>aaAA1234eo05</t>
+  </si>
+  <si>
+    <t>pakin</t>
+  </si>
+  <si>
+    <t>mser</t>
+  </si>
+  <si>
+    <t>lsflsf</t>
+  </si>
+  <si>
+    <t>sk4i</t>
+  </si>
+  <si>
+    <t>lf34d$4#$</t>
+  </si>
+  <si>
+    <t>injg4</t>
+  </si>
+  <si>
+    <t>sdf4rg</t>
+  </si>
+  <si>
+    <t>wf344</t>
+  </si>
+  <si>
+    <t>ret334</t>
+  </si>
+  <si>
+    <t>5t4f4r5Frfg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +102,13 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -136,9 +134,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,7 +457,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,89 +466,79 @@
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
+      <c r="F4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>